<commit_message>
Refreshing files and adding new image functionality
</commit_message>
<xml_diff>
--- a/Sentiment_Words.xlsx
+++ b/Sentiment_Words.xlsx
@@ -767,9 +767,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:S50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>